<commit_message>
example page in xlsx
</commit_message>
<xml_diff>
--- a/example and test case.xlsx
+++ b/example and test case.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6321557fa5c23060/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PythonProjects\excel-spaced-repetition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="314" documentId="8_{33B33D45-F7B9-45D9-9C93-F7BB648DEE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{19AC30B3-2D0A-4359-B85D-9AE2FD3F9D0D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E10260B-8B29-45E7-9C5D-5B52CE05F0B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E5F01474-DAEF-472A-BBDE-C0F04D68AA20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E5F01474-DAEF-472A-BBDE-C0F04D68AA20}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="input data 2" sheetId="3" r:id="rId2"/>
-    <sheet name="AFE_hidden_codesheet_49ddb8b8" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="Example" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="input data 2" sheetId="3" r:id="rId3"/>
+    <sheet name="AFE_hidden_codesheet_49ddb8b8" sheetId="2" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Day">Sheet1!$G$9</definedName>
+    <definedName name="day_to_review">Sheet1!$G$9</definedName>
     <definedName name="spacedr._get_review_intervals" xml:space="preserve"> _xlfn.LAMBDA(_xlpm.category_to_look,_xlpm.category_table,
     _xlfn.LET(
         _xlpm.category_table_first_column, INDEX(_xlpm.category_table,_xlfn.SEQUENCE(ROWS(_xlpm.category_table)),1),
@@ -77,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
   <si>
     <t>rows</t>
   </si>
@@ -224,6 +225,21 @@
   </si>
   <si>
     <t>Donec quis dui at dolor tempor interdum.</t>
+  </si>
+  <si>
+    <t>Open a server from start</t>
+  </si>
+  <si>
+    <t>Practice Eng. Page 3</t>
+  </si>
+  <si>
+    <t>Create an example of Pseucodode</t>
+  </si>
+  <si>
+    <t>initial date</t>
+  </si>
+  <si>
+    <t>is it time to review?</t>
   </si>
 </sst>
 </file>
@@ -433,28 +449,20 @@
     <cellStyle name="Title" xfId="10" builtinId="15"/>
     <cellStyle name="Title 2" xfId="2" xr:uid="{47C55C7B-CFDB-4AF7-BEC1-DA16BC913A50}"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+    </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
         <color theme="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -483,16 +491,16 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -508,11 +516,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DF5E6AA1-3006-4246-AD77-C54D5819AC83}" name="Table15" displayName="Table15" ref="B4:E8" totalsRowShown="0">
+  <autoFilter ref="B4:E8" xr:uid="{DF5E6AA1-3006-4246-AD77-C54D5819AC83}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{C6C0571E-AC34-4666-9C7A-F3200327DBC4}" name="task"/>
+    <tableColumn id="2" xr3:uid="{7EDE15B9-8170-4D2D-BBF2-7FB50E06D238}" name="category"/>
+    <tableColumn id="3" xr3:uid="{1986B9FC-8780-4056-984C-AF063466B344}" name="initial date" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{51FE4F55-6BEF-4E22-A6FD-84CBF205258C}" name="is it time to review?" dataDxfId="0">
+      <calculatedColumnFormula array="1">spacedr.its_time(day_to_review,Table15[[#This Row],[initial date]],Table15[[#This Row],[category]],AllCategories[])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{923EE402-DEA5-4B1C-BE24-27D4E195C794}" name="Table3" displayName="Table3" ref="L9:M22" totalsRowShown="0">
   <autoFilter ref="L9:M22" xr:uid="{923EE402-DEA5-4B1C-BE24-27D4E195C794}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{4E8A3A35-2FB3-45A0-AA74-99737C4744A1}" name="expected" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{19159F84-CE48-4CCF-86CF-55667BC9B3D8}" name="assert" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{4E8A3A35-2FB3-45A0-AA74-99737C4744A1}" name="expected" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{19159F84-CE48-4CCF-86CF-55667BC9B3D8}" name="assert" dataDxfId="7">
       <calculatedColumnFormula>#REF!=Table3[[#This Row],[expected]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -520,8 +543,8 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0B8E7C8B-09A1-4BD3-B040-50F66906945C}" name="Table2" displayName="Table2" ref="C25:I26" headerRowCount="0" totalsRowShown="0">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0B8E7C8B-09A1-4BD3-B040-50F66906945C}" name="AllCategories" displayName="AllCategories" ref="C25:I26" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{FA86E107-384B-4061-BD96-55D280438C1B}" name="nombre"/>
     <tableColumn id="2" xr3:uid="{E57E92E3-3E93-4CCF-A492-12BCF4B10E46}" name="días"/>
@@ -535,15 +558,15 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{52815E89-6D23-4A5C-99F1-2B8973A2A44A}" name="Table1" displayName="Table1" ref="C9:F22" totalsRowShown="0">
   <autoFilter ref="C9:F22" xr:uid="{52815E89-6D23-4A5C-99F1-2B8973A2A44A}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{15495644-CA8A-431E-8E37-6A01496AD120}" name="task"/>
     <tableColumn id="2" xr3:uid="{5A0EEEF3-792E-4025-9E77-06AD9B58F351}" name="category"/>
-    <tableColumn id="3" xr3:uid="{976C4074-D5CC-47D4-B315-8E4DF4B6154C}" name="date" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{58CCFF93-F5A7-4F14-B07A-801FF3C6388D}" name="is it time to review on →" dataDxfId="6">
-      <calculatedColumnFormula array="1">spacedr.its_time(Day,Table1[[#This Row],[date]],Table1[[#This Row],[category]],Table2[])</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{976C4074-D5CC-47D4-B315-8E4DF4B6154C}" name="date" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{58CCFF93-F5A7-4F14-B07A-801FF3C6388D}" name="is it time to review on →" dataDxfId="5">
+      <calculatedColumnFormula array="1">spacedr.its_time(day_to_review,Table1[[#This Row],[date]],Table1[[#This Row],[category]],AllCategories[])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -866,12 +889,126 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{073837F6-07F5-47E5-B77A-6B066A9A98CA}">
+  <dimension ref="B2:J8"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="43.42578125" customWidth="1"/>
+    <col min="6" max="6" width="37.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="4">
+        <v>44631</v>
+      </c>
+      <c r="E5" s="6" t="b" cm="1">
+        <f t="array" ref="E5">spacedr.its_time(day_to_review,Table15[[#This Row],[initial date]],Table15[[#This Row],[category]],AllCategories[])</f>
+        <v>1</v>
+      </c>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="4">
+        <v>44632</v>
+      </c>
+      <c r="E6" s="6" t="b" cm="1">
+        <f t="array" ref="E6">spacedr.its_time(day_to_review,Table15[[#This Row],[initial date]],Table15[[#This Row],[category]],AllCategories[])</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="4">
+        <v>44633</v>
+      </c>
+      <c r="E7" s="6" t="b" cm="1">
+        <f t="array" ref="E7">spacedr.its_time(day_to_review,Table15[[#This Row],[initial date]],Table15[[#This Row],[category]],AllCategories[])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="4">
+        <v>44635</v>
+      </c>
+      <c r="E8" s="6" t="b" cm="1">
+        <f t="array" ref="E8">spacedr.its_time(day_to_review,Table15[[#This Row],[initial date]],Table15[[#This Row],[category]],AllCategories[])</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E5:E8">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>INT(E5)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E30CA800-DC7F-474C-9C4C-476F4A68971C}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B4:T36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,7 +1088,7 @@
         <v>44631</v>
       </c>
       <c r="F10" s="6" t="b" cm="1">
-        <f t="array" ref="F10">spacedr.its_time(Day,Table1[[#This Row],[date]],Table1[[#This Row],[category]],Table2[])</f>
+        <f t="array" ref="F10">spacedr.its_time(day_to_review,Table1[[#This Row],[date]],Table1[[#This Row],[category]],AllCategories[])</f>
         <v>1</v>
       </c>
       <c r="H10" s="5"/>
@@ -981,7 +1118,7 @@
         <v>44632</v>
       </c>
       <c r="F11" s="6" t="b" cm="1">
-        <f t="array" ref="F11">spacedr.its_time(Day,Table1[[#This Row],[date]],Table1[[#This Row],[category]],Table2[])</f>
+        <f t="array" ref="F11">spacedr.its_time(day_to_review,Table1[[#This Row],[date]],Table1[[#This Row],[category]],AllCategories[])</f>
         <v>0</v>
       </c>
       <c r="H11" s="5"/>
@@ -1011,7 +1148,7 @@
         <v>44633</v>
       </c>
       <c r="F12" s="6" t="b" cm="1">
-        <f t="array" ref="F12">spacedr.its_time(Day,Table1[[#This Row],[date]],Table1[[#This Row],[category]],Table2[])</f>
+        <f t="array" ref="F12">spacedr.its_time(day_to_review,Table1[[#This Row],[date]],Table1[[#This Row],[category]],AllCategories[])</f>
         <v>0</v>
       </c>
       <c r="H12" s="5"/>
@@ -1041,7 +1178,7 @@
         <v>44634</v>
       </c>
       <c r="F13" s="6" t="b" cm="1">
-        <f t="array" ref="F13">spacedr.its_time(Day,Table1[[#This Row],[date]],Table1[[#This Row],[category]],Table2[])</f>
+        <f t="array" ref="F13">spacedr.its_time(day_to_review,Table1[[#This Row],[date]],Table1[[#This Row],[category]],AllCategories[])</f>
         <v>0</v>
       </c>
       <c r="H13" s="5"/>
@@ -1071,7 +1208,7 @@
         <v>44635</v>
       </c>
       <c r="F14" s="6" t="b" cm="1">
-        <f t="array" ref="F14">spacedr.its_time(Day,Table1[[#This Row],[date]],Table1[[#This Row],[category]],Table2[])</f>
+        <f t="array" ref="F14">spacedr.its_time(day_to_review,Table1[[#This Row],[date]],Table1[[#This Row],[category]],AllCategories[])</f>
         <v>1</v>
       </c>
       <c r="H14" s="5"/>
@@ -1101,7 +1238,7 @@
         <v>44636</v>
       </c>
       <c r="F15" s="6" t="b" cm="1">
-        <f t="array" ref="F15">spacedr.its_time(Day,Table1[[#This Row],[date]],Table1[[#This Row],[category]],Table2[])</f>
+        <f t="array" ref="F15">spacedr.its_time(day_to_review,Table1[[#This Row],[date]],Table1[[#This Row],[category]],AllCategories[])</f>
         <v>0</v>
       </c>
       <c r="H15" s="5"/>
@@ -1131,7 +1268,7 @@
         <v>44637</v>
       </c>
       <c r="F16" s="6" t="b" cm="1">
-        <f t="array" ref="F16">spacedr.its_time(Day,Table1[[#This Row],[date]],Table1[[#This Row],[category]],Table2[])</f>
+        <f t="array" ref="F16">spacedr.its_time(day_to_review,Table1[[#This Row],[date]],Table1[[#This Row],[category]],AllCategories[])</f>
         <v>1</v>
       </c>
       <c r="H16" s="5"/>
@@ -1161,7 +1298,7 @@
         <v>44638</v>
       </c>
       <c r="F17" s="6" t="b" cm="1">
-        <f t="array" ref="F17">spacedr.its_time(Day,Table1[[#This Row],[date]],Table1[[#This Row],[category]],Table2[])</f>
+        <f t="array" ref="F17">spacedr.its_time(day_to_review,Table1[[#This Row],[date]],Table1[[#This Row],[category]],AllCategories[])</f>
         <v>0</v>
       </c>
       <c r="H17" s="5"/>
@@ -1191,7 +1328,7 @@
         <v>44639</v>
       </c>
       <c r="F18" s="6" t="b" cm="1">
-        <f t="array" ref="F18">spacedr.its_time(Day,Table1[[#This Row],[date]],Table1[[#This Row],[category]],Table2[])</f>
+        <f t="array" ref="F18">spacedr.its_time(day_to_review,Table1[[#This Row],[date]],Table1[[#This Row],[category]],AllCategories[])</f>
         <v>0</v>
       </c>
       <c r="H18" s="5"/>
@@ -1221,7 +1358,7 @@
         <v>44640</v>
       </c>
       <c r="F19" s="6" t="b" cm="1">
-        <f t="array" ref="F19">spacedr.its_time(Day,Table1[[#This Row],[date]],Table1[[#This Row],[category]],Table2[])</f>
+        <f t="array" ref="F19">spacedr.its_time(day_to_review,Table1[[#This Row],[date]],Table1[[#This Row],[category]],AllCategories[])</f>
         <v>0</v>
       </c>
       <c r="H19" s="5"/>
@@ -1251,7 +1388,7 @@
         <v>44641</v>
       </c>
       <c r="F20" s="6" t="b" cm="1">
-        <f t="array" ref="F20">spacedr.its_time(Day,Table1[[#This Row],[date]],Table1[[#This Row],[category]],Table2[])</f>
+        <f t="array" ref="F20">spacedr.its_time(day_to_review,Table1[[#This Row],[date]],Table1[[#This Row],[category]],AllCategories[])</f>
         <v>0</v>
       </c>
       <c r="H20" s="5"/>
@@ -1281,7 +1418,7 @@
         <v>44642</v>
       </c>
       <c r="F21" s="6" t="b" cm="1">
-        <f t="array" ref="F21">spacedr.its_time(Day,Table1[[#This Row],[date]],Table1[[#This Row],[category]],Table2[])</f>
+        <f t="array" ref="F21">spacedr.its_time(day_to_review,Table1[[#This Row],[date]],Table1[[#This Row],[category]],AllCategories[])</f>
         <v>0</v>
       </c>
       <c r="H21" s="5"/>
@@ -1311,7 +1448,7 @@
         <v>44643</v>
       </c>
       <c r="F22" s="6" t="b" cm="1">
-        <f t="array" ref="F22">spacedr.its_time(Day,Table1[[#This Row],[date]],Table1[[#This Row],[category]],Table2[])</f>
+        <f t="array" ref="F22">spacedr.its_time(day_to_review,Table1[[#This Row],[date]],Table1[[#This Row],[category]],AllCategories[])</f>
         <v>0</v>
       </c>
       <c r="H22" s="5"/>
@@ -1463,10 +1600,10 @@
     <mergeCell ref="D24:I24"/>
   </mergeCells>
   <conditionalFormatting sqref="M10:M22">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>INT(M10)=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>INT(M10)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1480,7 +1617,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8396634B-F854-4DD5-9B26-EAD4D0CC5056}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1497,7 +1634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93FDB9A7-E5F4-4F0E-82BF-A43206BC6BAD}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F24"/>

</xml_diff>